<commit_message>
Add Decisition Tree Regression
</commit_message>
<xml_diff>
--- a/Performance Record.xlsx
+++ b/Performance Record.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="97">
   <si>
     <t>method\Route</t>
   </si>
@@ -32,38 +32,6 @@
     <t>Qlearning</t>
   </si>
   <si>
-    <t>0.743148171704
-chosenState:60</t>
-  </si>
-  <si>
-    <t>0.602564009072
-chosenState:62</t>
-  </si>
-  <si>
-    <t>0.997118570811
-chosenState:281</t>
-  </si>
-  <si>
-    <t>1
-chosenState:343</t>
-  </si>
-  <si>
-    <t>0.630193056034
-chosenState:73</t>
-  </si>
-  <si>
-    <t>0.695799585609
-chosenState:62</t>
-  </si>
-  <si>
-    <t>0.721296470146
-chosenState:62</t>
-  </si>
-  <si>
-    <t>0.741924483849
-chosenState:71</t>
-  </si>
-  <si>
     <t>BCN_BUD(0)</t>
   </si>
   <si>
@@ -86,62 +54,6 @@
   </si>
   <si>
     <t>SKP_MMX(7)</t>
-  </si>
-  <si>
-    <t>minimumPrice: 32.370952381
-maximumPrice: 126.656666667
-randomPrice: 48.593210526
-avgPredPrice: 41.4185714286
-performance: 14.76%</t>
-  </si>
-  <si>
-    <t>minimumPrice:11.3788888889
-maximumPrice:93.6011111111
-randomPrice: 53.0146969696
-avgPredPrice: 23.6011111111
-performance: 55.48%</t>
-  </si>
-  <si>
-    <t>minimumPrice:16.5284615385
-maximumPrice:90.5669230769
-randomPrice: 44.5160800000
-avgPredPrice: 37.2976923077
-performance: 16.22%</t>
-  </si>
-  <si>
-    <t>minimumPrice:9180.47619048
-maximumPrice:52799.5238095
-randomPrice: 14790.57368421(47)
-avgPredPrice: 13942.3809524
-performance: 5.73%</t>
-  </si>
-  <si>
-    <t>minimumPrice:155.153846154
-maximumPrice:843.615384615
-randomPrice: 380.874909090(45.6)
-avgPredPrice: 385.923076923
-performance: -1.33%</t>
-  </si>
-  <si>
-    <t>minimumPrice:58.4444444444
-maximumPrice:793.444444444
-randomPrice: 222.783939393(55.5)
-avgPredPrice: 90.3888888889
-performance: 59.43%</t>
-  </si>
-  <si>
-    <t>minimumPrice:1195.15384615
-maximumPrice:8583.61538462
-randomPrice: 3873.163111111(69.7)
-avgPredPrice: 2360.53846154
-performance: 39.05%</t>
-  </si>
-  <si>
-    <t>minimumPrice:1433.61538462
-maximumPrice:11556.6923077
-randomPrice: 3778.613454545(68.004)
-avgPredPrice: 2068.23076923
-performance: 45.26%</t>
   </si>
   <si>
     <r>
@@ -245,18 +157,6 @@
     <t>Detail Method Description</t>
   </si>
   <si>
-    <t>1. 13 input features: ( # feature 0~7: flight number dummy variables
-        # feature 8: departure date; feature 9: observed date state;
-        # feature 10: minimum price; feature 11: maximum price
-        # feature 12: current price)
-2. 1 output: the expected minimum price.
-3. Use 3-layer NN:  hidden layer with 6 units.
-4. Update method: nesterov_momentum, rate=0.002, update_momentum=0.4
-5. Use 20% as validation
-6. epoch = 100
-7. Datas without standardization</t>
-  </si>
-  <si>
     <t>1. 12 input features: ( # feature 0~7: flight number dummy variables
         # feature 8: departure date; feature 9: observed date state;
         # feature 10: minimum price; feature 11: maximum price)
@@ -293,12 +193,655 @@
 Normalized perfor = Performance / Max Perfor</t>
     </r>
   </si>
+  <si>
+    <t>Linear Regression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:11.3788888889
+maximumPrice:93.6011111111
+randomPrice: 53.0146969696
+avgPredPrice: 20.9622222222
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t>minimumPrice:25.8050769231
+maximumPrice:208.020461538
+randomPrice: 68.0150421818
+avgPredPrice: 
+Performance: 
+Max Perfor: 
+Normalized perfor:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:21.5127692308
+maximumPrice:154.505076923
+randomPrice: 69.716936
+avgPredPrice: 
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:14.6111111111
+maximumPrice:198.361111111
+randomPrice: 55.6959848485
+avgPredPrice: 
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t>minimumPrice:18.6184615385
+maximumPrice:101.233846154
+randomPrice:45.7049890909
+avgPredPrice:
+Performance: 
+Max Perfor: 
+Normalized perfor:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:16.5284615385
+maximumPrice:90.5669230769
+randomPrice: 44.5160800000
+avgPredPrice: 
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:11.3788888889
+maximumPrice:93.6011111111
+randomPrice: 53.0146969696
+avgPredPrice: 
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:29.3775238095
+maximumPrice:168.95847619
+randomPrice: 47.3298357895
+avgPredPrice:
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:29.3775238095
+maximumPrice:168.95847619
+randomPrice: 47.3298357895
+avgPredPrice:35.7775238095
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice: 32.370952381
+maximumPrice: 126.656666667
+randomPrice: 48.593210526
+avgPredPrice: 
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t>Linear Blending Regression  of NN Regression and Linear Regression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:16.5284615385
+maximumPrice:90.5669230769
+randomPrice: 44.5160800000
+avgPredPrice: 32.8746153846
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t>minimumPrice:18.6184615385
+maximumPrice:101.233846154
+randomPrice:45.7049890909
+avgPredPrice:25.5876923077
+Performance: 
+Max Perfor: 
+Normalized perfor:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:14.6111111111
+maximumPrice:198.361111111
+randomPrice: 55.6959848485
+avgPredPrice: 24.5416666667
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:21.5127692308
+maximumPrice:154.505076923
+randomPrice: 69.716936
+avgPredPrice: 40.1358461538
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t>minimumPrice:25.8050769231
+maximumPrice:208.020461538
+randomPrice: 68.0150421818
+avgPredPrice: 50.6589230769
+Performance: 
+Max Perfor: 
+Normalized perfor:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice: 32.370952381
+maximumPrice: 126.656666667
+randomPrice: 48.593210526
+avgPredPrice: 49.0376190476
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:29.3775238095
+maximumPrice:168.95847619
+randomPrice: 47.3298357895
+avgPredPrice:106.482285714
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:11.3788888889
+maximumPrice:93.6011111111
+randomPrice: 53.0146969696
+avgPredPrice: 28.1844444444
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:16.5284615385
+maximumPrice:90.5669230769
+randomPrice: 44.5160800000
+avgPredPrice: 46.7207692308
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t>minimumPrice:18.6184615385
+maximumPrice:101.233846154
+randomPrice:45.7049890909
+avgPredPrice:57.0646153846
+Performance: 
+Max Perfor: 
+Normalized perfor:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:14.6111111111
+maximumPrice:198.361111111
+randomPrice: 55.6959848485
+avgPredPrice:81.625
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:21.5127692308
+maximumPrice:154.505076923
+randomPrice: 69.716936
+avgPredPrice:81.4666153846
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t>minimumPrice:25.8050769231
+maximumPrice:208.020461538
+randomPrice: 68.0150421818
+avgPredPrice:146.058923077
+Performance: 
+Max Perfor: 
+Normalized perfor:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice: 32.370952381
+maximumPrice: 126.656666667
+randomPrice: 48.593210526
+avgPredPrice: 41.4185714286
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:9180.47619048
+maximumPrice:52799.5238095
+randomPrice: 14790.57368421(47)
+avgPredPrice: 13942.3809524
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:11.3788888889
+maximumPrice:93.6011111111
+randomPrice: 53.0146969696
+avgPredPrice: 23.6011111111
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:16.5284615385
+maximumPrice:90.5669230769
+randomPrice: 44.5160800000
+avgPredPrice: 37.2976923077
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:155.153846154
+maximumPrice:843.615384615
+randomPrice: 380.874909090(45.6)
+avgPredPrice: 385.923076923
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:58.4444444444
+maximumPrice:793.444444444
+randomPrice: 222.783939393(55.5)
+avgPredPrice: 90.3888888889
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:1195.15384615
+maximumPrice:8583.61538462
+randomPrice: 3873.163111111(69.7)
+avgPredPrice: 2360.53846154
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:1433.61538462
+maximumPrice:11556.6923077
+randomPrice: 3778.613454545(68.004)
+avgPredPrice: 2068.23076923
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t>1. Objective function is mean squared error
+2. it is just a least-square problem
+3. we found the prediction is lower than the real expected minimum price</t>
+  </si>
+  <si>
+    <t>1. 13 input features: ( # feature 0~7: flight number dummy variables
+        # feature 8: departure date; feature 9: observed date state;
+        # feature 10: minimum price; feature 11: maximum price
+        # feature 12: current price)
+2. 1 output: the expected minimum price.
+3. Use 3-layer NN:  hidden layer with 6 units.
+4. Update method: nesterov_momentum, rate=0.002, update_momentum=0.4
+5. Use 20% as validation
+6. epoch = 100
+7. Datas without standardization
+8. We found that the prediction minimum price is higher than the real minimum price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:21.5127692308
+maximumPrice:154.505076923
+randomPrice: 69.716936
+avgPredPrice: 39.3050769231
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:29.3775238095
+maximumPrice:168.95847619
+randomPrice: 47.3298357895
+avgPredPrice:41.8727619048
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t>Decision Tree Regression with max depth = 4
+price tolerance = 5
+(i.e. the predicted price +5 larger than current price -&gt; buy)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice: 32.370952381
+maximumPrice: 126.656666667
+randomPrice: 48.593210526
+avgPredPrice: 47.609047619
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:29.3775238095
+maximumPrice:168.95847619
+randomPrice: 47.3298357895
+avgPredPrice:42.0251428571
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t>minimumPrice:18.6184615385
+maximumPrice:101.233846154
+randomPrice:45.7049890909
+avgPredPrice:26.4184615385
+Performance: 
+Max Perfor: 
+Normalized perfor:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:14.6111111111
+maximumPrice:198.361111111
+randomPrice: 55.6959848485
+avgPredPrice: 22.6666666667
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t>minimumPrice:25.8050769231
+maximumPrice:208.020461538
+randomPrice: 68.0150421818
+avgPredPrice: 47.6127692308
+Performance: 
+Max Perfor: 
+Normalized perfor:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice: 32.370952381
+maximumPrice: 126.656666667
+randomPrice: 48.593210526
+avgPredPrice: 39.5138095238
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:11.3788888889
+maximumPrice:93.6011111111
+randomPrice: 53.0146969696
+avgPredPrice: 20.1288888889
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:16.5284615385
+maximumPrice:90.5669230769
+randomPrice: 44.5160800000
+avgPredPrice: 32.2976923077
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t>minimumPrice:18.6184615385
+maximumPrice:101.233846154
+randomPrice:45.7049890909
+avgPredPrice:24.3415384615
+Performance: 
+Max Perfor: 
+Normalized perfor:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:14.6111111111
+maximumPrice:198.361111111
+randomPrice: 55.6959848485
+avgPredPrice: 24.1944444444
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:21.5127692308
+maximumPrice:154.505076923
+randomPrice: 69.716936
+avgPredPrice: 41.382
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t>minimumPrice:25.8050769231
+maximumPrice:208.020461538
+randomPrice: 68.0150421818
+avgPredPrice: 44.982
+Performance: 
+Max Perfor: 
+Normalized perfor:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice: 32.370952381
+maximumPrice: 126.656666667
+randomPrice: 48.593210526
+avgPredPrice: 69.99
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:29.3775238095
+maximumPrice:168.95847619
+randomPrice: 47.3298357895
+avgPredPrice:43.7013333333
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:11.3788888889
+maximumPrice:93.6011111111
+randomPrice: 53.0146969696
+avgPredPrice: 18.1844444444
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:16.5284615385
+maximumPrice:90.5669230769
+randomPrice: 44.5160800000
+avgPredPrice: 30.1823076923
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t>minimumPrice:18.6184615385
+maximumPrice:101.233846154
+randomPrice:45.7049890909
+avgPredPrice:29.9261538462
+Performance: 
+Max Perfor: 
+Normalized perfor:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:14.6111111111
+maximumPrice:198.361111111
+randomPrice: 55.6959848485
+avgPredPrice: 23.5
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:21.5127692308
+maximumPrice:154.505076923
+randomPrice: 69.716936
+avgPredPrice: 40.9666153846
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t>minimumPrice:25.8050769231
+maximumPrice:208.020461538
+randomPrice: 68.0150421818
+avgPredPrice: 48.4435384615
+Performance: 
+Max Perfor: 
+Normalized perfor:</t>
+  </si>
+  <si>
+    <t>Decision Tree Regression with max depth = 2
+price tolerance = 5
+(i.e. the predicted price +5 larger than current price -&gt; buy)</t>
+  </si>
+  <si>
+    <t>Decision Tree Regression with max depth = 3
+price tolerance = 5
+(i.e. the predicted price +5 larger than current price -&gt; buy)</t>
+  </si>
+  <si>
+    <t>Decision Tree Regression with max depth = 5
+price tolerance = 5
+(i.e. the predicted price +5 larger than current price -&gt; buy)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice: 32.370952381
+maximumPrice: 126.656666667
+randomPrice: 48.593210526
+avgPredPrice: 44.7519047619
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:29.3775238095
+maximumPrice:168.95847619
+randomPrice: 47.3298357895
+avgPredPrice:44.3108571429
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:16.5284615385
+maximumPrice:90.5669230769
+randomPrice: 44.5160800000
+avgPredPrice: 28.4515384615
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:21.5127692308
+maximumPrice:154.505076923
+randomPrice: 69.716936
+avgPredPrice: 42.8358461538
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t>minimumPrice:25.8050769231
+maximumPrice:208.020461538
+randomPrice: 68.0150421818
+avgPredPrice: 56.5435384615
+Performance: 
+Max Perfor: 
+Normalized perfor:</t>
+  </si>
+  <si>
+    <t>Decision Tree Regression with max depth = 6
+price tolerance = 5
+(i.e. the predicted price +5 larger than current price -&gt; buy)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice: 32.370952381
+maximumPrice: 126.656666667
+randomPrice: 48.593210526
+avgPredPrice: 47.1328571429
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:29.3775238095
+maximumPrice:168.95847619
+randomPrice: 47.3298357895
+avgPredPrice:33.3394285714
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:11.3788888889
+maximumPrice:93.6011111111
+randomPrice: 53.0146969696
+avgPredPrice: 19.5733333333
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:16.5284615385
+maximumPrice:90.5669230769
+randomPrice: 44.5160800000
+avgPredPrice: 28.2592307692
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t>minimumPrice:18.6184615385
+maximumPrice:101.233846154
+randomPrice:45.7049890909
+avgPredPrice:24.8030769231
+Performance: 
+Max Perfor: 
+Normalized perfor:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice:21.5127692308
+maximumPrice:154.505076923
+randomPrice: 69.716936
+avgPredPrice: 41.5896923077
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
+  <si>
+    <t>minimumPrice:25.8050769231
+maximumPrice:208.020461538
+randomPrice: 68.0150421818
+avgPredPrice: 65.6127692308
+Performance: 
+Max Perfor: 
+Normalized perfor:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumPrice: 32.370952381
+maximumPrice: 126.656666667
+randomPrice: 48.593210526
+avgPredPrice: 80.9423809524
+Performance: 
+Max Perfor: 
+Normalized perfor: </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -341,6 +884,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -364,13 +915,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -650,11 +1205,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -674,128 +1227,344 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:10" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="197" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="2" t="s">
+    </row>
+    <row r="7" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="E9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="H17" s="3"/>
+    </row>
+    <row r="19" spans="2:9" ht="112" x14ac:dyDescent="0.2">
+      <c r="B19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="181" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H17" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add uniform blending classification
</commit_message>
<xml_diff>
--- a/Performance Record.xlsx
+++ b/Performance Record.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24500" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="489">
   <si>
     <r>
       <rPr>
@@ -45092,12 +45092,184 @@
     <t>Average Performance: 17.14%
 Average Normalized Performance: 48.27%</t>
   </si>
+  <si>
+    <t>TRAIN:
+minimumPrice: 44.4344444444
+maximumPrice: 115.915925926
+randomPrice: 68.4391315136
+avgPredPrice: 47.3974074074
+Performance: 30.75%
+Max Perfor: 35.07%
+Normalized perfor: 87.66%</t>
+  </si>
+  <si>
+    <t>TRAIN:
+minimumPrice: 38.9605925926
+maximumPrice: 126.782814815
+randomPrice: 67.4260645161
+avgPredPrice: 41.2124444444
+Performance: 38.88%
+Max Perfor: 42.22%
+Normalized perfor: 92.09%</t>
+  </si>
+  <si>
+    <t>TRAIN:
+minimumPrice: 68.6566666667
+maximumPrice: 144.212222222
+randomPrice: 93.2808545727
+avgPredPrice: 75.1011111111
+Performance: 19.49%
+Max Perfor: 26.4%
+Normalized perfor: 73.83%</t>
+  </si>
+  <si>
+    <t>TRAIN:
+minimumPrice: 49.6566666667
+maximumPrice: 129.656666667
+randomPrice: 77.4751720047
+avgPredPrice: 53.6566666667
+Performance: 30.74%
+Max Perfor: 35.91%
+Normalized perfor: 85.62%</t>
+  </si>
+  <si>
+    <t>TRAIN:
+minimumPrice: 48.2691891892
+maximumPrice: 141.252972973
+randomPrice: 75.0340018399
+avgPredPrice: 54.2691891892
+Performance: 27.67%
+Max Perfor: 35.67%
+Normalized perfor: 77.58%</t>
+  </si>
+  <si>
+    <t>TRAIN:
+minimumPrice: 47.0833333333
+maximumPrice: 149.972222222
+randomPrice: 73.9964736451
+avgPredPrice: 48.6388888889
+Performance: 34.27%
+Max Perfor: 36.37%
+Normalized perfor: 94.22%</t>
+  </si>
+  <si>
+    <t>TRAIN:
+minimumPrice: 68.982
+maximumPrice: 174.402
+randomPrice: 105.280932384
+avgPredPrice: 70.242
+Performance: 33.28%
+Max Perfor: 34.48%
+Normalized perfor: 96.53%</t>
+  </si>
+  <si>
+    <t>TRAIN:
+minimumPrice: 63.1279459459
+maximumPrice: 160.91172973
+randomPrice: 97.1720369004
+avgPredPrice: 68.8684864865
+Performance: 29.13%
+Max Perfor: 35.03%
+Normalized perfor: 83.14%</t>
+  </si>
+  <si>
+    <t>Average Performance: 30.53%
+Average Normalized Performance: 86.33%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 32.370952381
+maximumPrice: 126.656666667
+randomPrice: 55.4820634921
+avgPredPrice: 41.4185714286
+Performance: 25.35%
+Max Perfor: 41.66%
+Normalized perfor: 60.85%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 29.3775238095
+maximumPrice: 168.95847619
+randomPrice: 57.8067301587
+avgPredPrice: 42.3299047619
+Performance: 26.77%
+Max Perfor: 49.18%
+Normalized perfor: 54.44%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 11.3788888889
+maximumPrice: 93.6011111111
+randomPrice: 23.152037037
+avgPredPrice: 19.2955555556
+Performance: 16.66%
+Max Perfor: 50.85%
+Normalized perfor: 32.76%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 16.5284615385
+maximumPrice: 90.5669230769
+randomPrice: 33.3727319588
+avgPredPrice: 32.2976923077
+Performance: 3.22%
+Max Perfor: 50.47%
+Normalized perfor: 6.38%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 18.6184615385
+maximumPrice: 101.233846154
+randomPrice: 35.3032044199
+avgPredPrice: 25.7723076923
+Performance: 27.0%
+Max Perfor: 47.26%
+Normalized perfor: 57.12%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 14.6111111111
+maximumPrice: 198.361111111
+randomPrice: 41.1180555556
+avgPredPrice: 19.9583333333
+Performance: 51.46%
+Max Perfor: 64.47%
+Normalized perfor: 79.83%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 21.5127692308
+maximumPrice: 154.505076923
+randomPrice: 56.3433402062
+avgPredPrice: 36.4666153846
+Performance: 35.28%
+Max Perfor: 61.82%
+Normalized perfor: 57.07%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 25.8050769231
+maximumPrice: 208.020461538
+randomPrice: 60.2546519337
+avgPredPrice: 38.0589230769
+Performance: 36.84%
+Max Perfor: 57.17%
+Normalized perfor: 64.43%</t>
+  </si>
+  <si>
+    <t>Average Performance: 27.82%
+Average Normalized Performance: 51.61%</t>
+  </si>
+  <si>
+    <t>Uniform Blending
+logistic regression, AdaBoost with Decision Tree, KNN, Decision Tree, Neural Network</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="65" x14ac:knownFonts="1">
+  <fonts count="66" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -45534,6 +45706,12 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -45562,7 +45740,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -45672,13 +45850,22 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -45959,10 +46146,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K68"/>
+  <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="82" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="82" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -46091,7 +46278,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="161" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="43" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -46457,7 +46644,7 @@
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="41" t="s">
         <v>461</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -46490,7 +46677,7 @@
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="43"/>
+      <c r="A18" s="42"/>
       <c r="B18" s="5" t="s">
         <v>451</v>
       </c>
@@ -46500,7 +46687,7 @@
       <c r="D18" s="5" t="s">
         <v>453</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="10" t="s">
         <v>454</v>
       </c>
       <c r="F18" s="5" t="s">
@@ -46520,1128 +46707,1192 @@
       </c>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
+    <row r="19" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="45" t="s">
+        <v>488</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="E19" s="44" t="s">
+        <v>473</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>478</v>
+      </c>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" ht="154" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
-        <v>135</v>
-      </c>
+    <row r="20" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="46"/>
       <c r="B20" s="5" t="s">
-        <v>136</v>
+        <v>479</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>137</v>
+        <v>480</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>139</v>
+        <v>481</v>
+      </c>
+      <c r="E20" s="44" t="s">
+        <v>482</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>140</v>
+        <v>483</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>141</v>
+        <v>484</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>142</v>
+        <v>485</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="J20" s="5"/>
+        <v>486</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>487</v>
+      </c>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" ht="167" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
-      <c r="B21" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="J21" s="6"/>
-      <c r="K21" s="1" t="s">
-        <v>152</v>
-      </c>
+    <row r="21" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" ht="169" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="40" t="s">
-        <v>153</v>
+    <row r="22" spans="1:11" ht="154" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="39" t="s">
+        <v>135</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11" ht="133" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
-      <c r="B23" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="H23" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="I23" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="J23" s="13"/>
+    <row r="23" spans="1:11" ht="167" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="29"/>
+      <c r="B23" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="J23" s="6"/>
       <c r="K23" s="1" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="169" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="40" t="s">
-        <v>171</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
+        <v>153</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="J24" s="5"/>
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:11" ht="133" x14ac:dyDescent="0.25">
       <c r="A25" s="35"/>
-      <c r="B25" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="J25" s="5"/>
-      <c r="K25" s="20"/>
+      <c r="B25" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="J25" s="13"/>
+      <c r="K25" s="1" t="s">
+        <v>170</v>
+      </c>
     </row>
-    <row r="26" spans="1:11" ht="152" x14ac:dyDescent="0.25">
-      <c r="A26" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="J26" s="5"/>
-      <c r="K26" s="20"/>
+    <row r="26" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A26" s="40" t="s">
+        <v>171</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
     </row>
     <row r="27" spans="1:11" ht="133" x14ac:dyDescent="0.25">
       <c r="A27" s="35"/>
-      <c r="B27" s="10" t="s">
-        <v>189</v>
+      <c r="B27" s="5" t="s">
+        <v>172</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="20"/>
     </row>
     <row r="28" spans="1:11" ht="152" x14ac:dyDescent="0.25">
-      <c r="A28" s="36" t="s">
-        <v>197</v>
+      <c r="A28" s="34" t="s">
+        <v>180</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" ht="182" x14ac:dyDescent="0.3">
-      <c r="A29" s="29"/>
-      <c r="B29" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="H29" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I29" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="J29" s="8"/>
+    <row r="29" spans="1:11" ht="133" x14ac:dyDescent="0.25">
+      <c r="A29" s="35"/>
+      <c r="B29" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="J29" s="5"/>
       <c r="K29" s="20"/>
     </row>
     <row r="30" spans="1:11" ht="152" x14ac:dyDescent="0.25">
-      <c r="A30" s="34" t="s">
-        <v>214</v>
+      <c r="A30" s="36" t="s">
+        <v>197</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" ht="133" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="182" x14ac:dyDescent="0.3">
       <c r="A31" s="29"/>
-      <c r="B31" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="J31" s="5"/>
+      <c r="B31" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="J31" s="8"/>
       <c r="K31" s="20"/>
     </row>
     <row r="32" spans="1:11" ht="152" x14ac:dyDescent="0.25">
-      <c r="A32" s="37" t="s">
-        <v>231</v>
+      <c r="A32" s="34" t="s">
+        <v>214</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="J32" s="5"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" ht="182" x14ac:dyDescent="0.3">
-      <c r="A33" s="38"/>
-      <c r="B33" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>245</v>
-      </c>
-      <c r="H33" s="8" t="s">
-        <v>246</v>
-      </c>
-      <c r="I33" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="J33" s="8"/>
+    <row r="33" spans="1:11" ht="133" x14ac:dyDescent="0.25">
+      <c r="A33" s="29"/>
+      <c r="B33" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="J33" s="5"/>
       <c r="K33" s="20"/>
     </row>
     <row r="34" spans="1:11" ht="152" x14ac:dyDescent="0.25">
-      <c r="A34" s="34" t="s">
-        <v>248</v>
+      <c r="A34" s="37" t="s">
+        <v>231</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>253</v>
+        <v>236</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>254</v>
+        <v>237</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
       <c r="J34" s="5"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" ht="133" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
-      <c r="B35" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="I35" s="10" t="s">
-        <v>264</v>
-      </c>
-      <c r="J35" s="10"/>
+    <row r="35" spans="1:11" ht="182" x14ac:dyDescent="0.3">
+      <c r="A35" s="38"/>
+      <c r="B35" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="J35" s="8"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" ht="162" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="28" t="s">
-        <v>265</v>
+    <row r="36" spans="1:11" ht="152" x14ac:dyDescent="0.25">
+      <c r="A36" s="34" t="s">
+        <v>248</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="J36" s="5"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" ht="182" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="133" x14ac:dyDescent="0.25">
       <c r="A37" s="29"/>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="I37" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="J37" s="10"/>
+      <c r="K37" s="20"/>
+    </row>
+    <row r="38" spans="1:11" ht="162" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="28" t="s">
+        <v>265</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="J38" s="5"/>
+      <c r="K38" s="20"/>
+    </row>
+    <row r="39" spans="1:11" ht="182" x14ac:dyDescent="0.3">
+      <c r="A39" s="29"/>
+      <c r="B39" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C39" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D39" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E39" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="F39" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="G37" s="8" t="s">
+      <c r="G39" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="H37" s="8" t="s">
+      <c r="H39" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="I37" s="8" t="s">
+      <c r="I39" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="J37" s="8"/>
-      <c r="K37" s="23" t="s">
+      <c r="J39" s="8"/>
+      <c r="K39" s="23" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="163" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="30" t="s">
+    <row r="40" spans="1:11" ht="163" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="30" t="s">
         <v>282</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B40" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C40" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D40" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="E40" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="F40" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="G38" s="5" t="s">
+      <c r="G40" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="H38" s="5" t="s">
+      <c r="H40" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="I38" s="5" t="s">
+      <c r="I40" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="J38" s="5"/>
-      <c r="K38" s="23"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="23"/>
     </row>
-    <row r="39" spans="1:11" ht="133" x14ac:dyDescent="0.25">
-      <c r="A39" s="29"/>
-      <c r="B39" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="J39" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="K39" s="22"/>
-    </row>
-    <row r="40" spans="1:11" ht="146" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="30" t="s">
-        <v>300</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="I40" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="J40" s="5"/>
-      <c r="K40" s="22"/>
-    </row>
-    <row r="41" spans="1:11" ht="149" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="133" x14ac:dyDescent="0.25">
       <c r="A41" s="29"/>
       <c r="B41" s="5" t="s">
-        <v>309</v>
+        <v>291</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>310</v>
+        <v>292</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>311</v>
+        <v>293</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>312</v>
+        <v>294</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>313</v>
+        <v>295</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>316</v>
+        <v>298</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="K41" s="22"/>
     </row>
-    <row r="42" spans="1:11" ht="129" x14ac:dyDescent="0.25">
-      <c r="A42" s="31" t="s">
+    <row r="42" spans="1:11" ht="146" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="30" t="s">
+        <v>300</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="J42" s="5"/>
+      <c r="K42" s="22"/>
+    </row>
+    <row r="43" spans="1:11" ht="149" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="29"/>
+      <c r="B43" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="K43" s="22"/>
+    </row>
+    <row r="44" spans="1:11" ht="129" x14ac:dyDescent="0.25">
+      <c r="A44" s="31" t="s">
         <v>318</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B44" s="15" t="s">
         <v>319</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="C44" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="D44" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="E42" s="15" t="s">
+      <c r="E44" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="F42" s="15" t="s">
+      <c r="F44" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G42" s="15" t="s">
+      <c r="G44" s="15" t="s">
         <v>324</v>
       </c>
-      <c r="H42" s="15" t="s">
+      <c r="H44" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="I42" s="15" t="s">
+      <c r="I44" s="15" t="s">
         <v>326</v>
       </c>
-      <c r="J42" s="19" t="s">
+      <c r="J44" s="19" t="s">
         <v>327</v>
       </c>
-      <c r="K42" s="13" t="s">
+      <c r="K44" s="13" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="131" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="29"/>
-      <c r="B43" s="15" t="s">
+    <row r="45" spans="1:11" ht="131" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="29"/>
+      <c r="B45" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="C45" s="15" t="s">
         <v>329</v>
       </c>
-      <c r="D43" s="15" t="s">
+      <c r="D45" s="15" t="s">
         <v>330</v>
       </c>
-      <c r="E43" s="15" t="s">
+      <c r="E45" s="15" t="s">
         <v>331</v>
       </c>
-      <c r="F43" s="15" t="s">
+      <c r="F45" s="15" t="s">
         <v>332</v>
       </c>
-      <c r="G43" s="15" t="s">
+      <c r="G45" s="15" t="s">
         <v>333</v>
       </c>
-      <c r="H43" s="15" t="s">
+      <c r="H45" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="I43" s="15" t="s">
+      <c r="I45" s="15" t="s">
         <v>335</v>
       </c>
-      <c r="J43" s="19" t="s">
+      <c r="J45" s="19" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="128" x14ac:dyDescent="0.2">
-      <c r="A44" s="32" t="s">
+    <row r="46" spans="1:11" ht="128" x14ac:dyDescent="0.2">
+      <c r="A46" s="32" t="s">
         <v>337</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B46" s="15" t="s">
         <v>338</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="C46" s="15" t="s">
         <v>339</v>
       </c>
-      <c r="D44" s="15" t="s">
+      <c r="D46" s="15" t="s">
         <v>340</v>
       </c>
-      <c r="E44" s="15" t="s">
+      <c r="E46" s="15" t="s">
         <v>341</v>
       </c>
-      <c r="F44" s="15" t="s">
+      <c r="F46" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="G44" s="15" t="s">
+      <c r="G46" s="15" t="s">
         <v>343</v>
       </c>
-      <c r="H44" s="16" t="s">
+      <c r="H46" s="16" t="s">
         <v>344</v>
       </c>
-      <c r="I44" s="15" t="s">
+      <c r="I46" s="15" t="s">
         <v>345</v>
       </c>
-      <c r="J44" s="19" t="s">
+      <c r="J46" s="19" t="s">
         <v>346</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="144" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="33"/>
-      <c r="B45" s="17" t="s">
-        <v>347</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>348</v>
-      </c>
-      <c r="D45" s="17" t="s">
-        <v>349</v>
-      </c>
-      <c r="E45" s="17" t="s">
-        <v>350</v>
-      </c>
-      <c r="F45" s="17" t="s">
-        <v>351</v>
-      </c>
-      <c r="G45" s="17" t="s">
-        <v>352</v>
-      </c>
-      <c r="H45" s="17" t="s">
-        <v>353</v>
-      </c>
-      <c r="I45" s="17" t="s">
-        <v>354</v>
-      </c>
-      <c r="J45" s="24" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="144" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="26" t="s">
-        <v>356</v>
-      </c>
-      <c r="B46" s="18" t="s">
-        <v>357</v>
-      </c>
-      <c r="C46" s="18" t="s">
-        <v>358</v>
-      </c>
-      <c r="D46" s="18" t="s">
-        <v>359</v>
-      </c>
-      <c r="E46" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="F46" s="18" t="s">
-        <v>361</v>
-      </c>
-      <c r="G46" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="H46" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="I46" s="18" t="s">
-        <v>364</v>
-      </c>
-      <c r="J46" s="21" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="144" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="26"/>
-      <c r="B47" s="18" t="s">
-        <v>366</v>
-      </c>
-      <c r="C47" s="18" t="s">
-        <v>367</v>
-      </c>
-      <c r="D47" s="18" t="s">
-        <v>368</v>
-      </c>
-      <c r="E47" s="18" t="s">
-        <v>369</v>
-      </c>
-      <c r="F47" s="18" t="s">
-        <v>370</v>
-      </c>
-      <c r="G47" s="18" t="s">
-        <v>371</v>
-      </c>
-      <c r="H47" s="18" t="s">
-        <v>372</v>
-      </c>
-      <c r="I47" s="18" t="s">
-        <v>373</v>
-      </c>
-      <c r="J47" s="21" t="s">
-        <v>374</v>
+      <c r="A47" s="33"/>
+      <c r="B47" s="17" t="s">
+        <v>347</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>348</v>
+      </c>
+      <c r="D47" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="E47" s="17" t="s">
+        <v>350</v>
+      </c>
+      <c r="F47" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="G47" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="H47" s="17" t="s">
+        <v>353</v>
+      </c>
+      <c r="I47" s="17" t="s">
+        <v>354</v>
+      </c>
+      <c r="J47" s="24" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="144" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="26" t="s">
-        <v>375</v>
+        <v>356</v>
       </c>
       <c r="B48" s="18" t="s">
-        <v>376</v>
+        <v>357</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>377</v>
+        <v>358</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>378</v>
+        <v>359</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>379</v>
+        <v>360</v>
       </c>
       <c r="F48" s="18" t="s">
-        <v>380</v>
+        <v>361</v>
       </c>
       <c r="G48" s="18" t="s">
-        <v>381</v>
+        <v>362</v>
       </c>
       <c r="H48" s="18" t="s">
-        <v>382</v>
+        <v>363</v>
       </c>
       <c r="I48" s="18" t="s">
-        <v>383</v>
+        <v>364</v>
       </c>
       <c r="J48" s="21" t="s">
-        <v>384</v>
+        <v>365</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="144" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="26"/>
       <c r="B49" s="18" t="s">
-        <v>385</v>
+        <v>366</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>386</v>
+        <v>367</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>387</v>
+        <v>368</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>388</v>
+        <v>369</v>
       </c>
       <c r="F49" s="18" t="s">
-        <v>389</v>
+        <v>370</v>
       </c>
       <c r="G49" s="18" t="s">
-        <v>390</v>
+        <v>371</v>
       </c>
       <c r="H49" s="18" t="s">
-        <v>391</v>
+        <v>372</v>
       </c>
       <c r="I49" s="18" t="s">
-        <v>392</v>
+        <v>373</v>
       </c>
       <c r="J49" s="21" t="s">
-        <v>393</v>
+        <v>374</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="144" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="26" t="s">
-        <v>394</v>
+        <v>375</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>395</v>
+        <v>376</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>396</v>
+        <v>377</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>397</v>
+        <v>378</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>398</v>
+        <v>379</v>
       </c>
       <c r="F50" s="18" t="s">
-        <v>399</v>
+        <v>380</v>
       </c>
       <c r="G50" s="18" t="s">
-        <v>400</v>
+        <v>381</v>
       </c>
       <c r="H50" s="18" t="s">
-        <v>401</v>
+        <v>382</v>
       </c>
       <c r="I50" s="18" t="s">
-        <v>402</v>
+        <v>383</v>
       </c>
       <c r="J50" s="21" t="s">
-        <v>403</v>
+        <v>384</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="128" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" ht="144" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="26"/>
       <c r="B51" s="18" t="s">
-        <v>404</v>
+        <v>385</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>405</v>
+        <v>386</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>406</v>
+        <v>387</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>407</v>
+        <v>388</v>
       </c>
       <c r="F51" s="18" t="s">
-        <v>408</v>
+        <v>389</v>
       </c>
       <c r="G51" s="18" t="s">
-        <v>409</v>
+        <v>390</v>
       </c>
       <c r="H51" s="18" t="s">
-        <v>410</v>
-      </c>
-      <c r="I51" s="25" t="s">
-        <v>411</v>
-      </c>
-      <c r="J51" s="19" t="s">
-        <v>412</v>
+        <v>391</v>
+      </c>
+      <c r="I51" s="18" t="s">
+        <v>392</v>
+      </c>
+      <c r="J51" s="21" t="s">
+        <v>393</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="26" x14ac:dyDescent="0.3">
-      <c r="A52" s="11" t="s">
-        <v>413</v>
-      </c>
-      <c r="B52" s="19"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="19"/>
-      <c r="H52" s="19"/>
-      <c r="I52" s="19"/>
-      <c r="J52" s="19"/>
+    <row r="52" spans="1:10" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="26" t="s">
+        <v>394</v>
+      </c>
+      <c r="B52" s="18" t="s">
+        <v>395</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>396</v>
+      </c>
+      <c r="D52" s="18" t="s">
+        <v>397</v>
+      </c>
+      <c r="E52" s="18" t="s">
+        <v>398</v>
+      </c>
+      <c r="F52" s="18" t="s">
+        <v>399</v>
+      </c>
+      <c r="G52" s="18" t="s">
+        <v>400</v>
+      </c>
+      <c r="H52" s="18" t="s">
+        <v>401</v>
+      </c>
+      <c r="I52" s="18" t="s">
+        <v>402</v>
+      </c>
+      <c r="J52" s="21" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="53" spans="1:10" ht="128" x14ac:dyDescent="0.2">
-      <c r="A53" s="27" t="s">
+      <c r="A53" s="26"/>
+      <c r="B53" s="18" t="s">
+        <v>404</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>405</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>406</v>
+      </c>
+      <c r="E53" s="18" t="s">
+        <v>407</v>
+      </c>
+      <c r="F53" s="18" t="s">
+        <v>408</v>
+      </c>
+      <c r="G53" s="18" t="s">
+        <v>409</v>
+      </c>
+      <c r="H53" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="I53" s="25" t="s">
+        <v>411</v>
+      </c>
+      <c r="J53" s="19" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="26" x14ac:dyDescent="0.3">
+      <c r="A54" s="11" t="s">
+        <v>413</v>
+      </c>
+      <c r="B54" s="19"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="19"/>
+      <c r="J54" s="19"/>
+    </row>
+    <row r="55" spans="1:10" ht="128" x14ac:dyDescent="0.2">
+      <c r="A55" s="27" t="s">
         <v>414</v>
       </c>
-      <c r="B53" s="18" t="s">
+      <c r="B55" s="18" t="s">
         <v>415</v>
       </c>
-      <c r="C53" s="18" t="s">
+      <c r="C55" s="18" t="s">
         <v>416</v>
       </c>
-      <c r="D53" s="18" t="s">
+      <c r="D55" s="18" t="s">
         <v>417</v>
       </c>
-      <c r="E53" s="18" t="s">
+      <c r="E55" s="18" t="s">
         <v>418</v>
       </c>
-      <c r="F53" s="18" t="s">
+      <c r="F55" s="18" t="s">
         <v>419</v>
       </c>
-      <c r="G53" s="18" t="s">
+      <c r="G55" s="18" t="s">
         <v>420</v>
       </c>
-      <c r="H53" s="18" t="s">
+      <c r="H55" s="18" t="s">
         <v>421</v>
       </c>
-      <c r="I53" s="18" t="s">
+      <c r="I55" s="18" t="s">
         <v>422</v>
       </c>
-      <c r="J53" s="19" t="s">
+      <c r="J55" s="19" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="137" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="27"/>
-      <c r="B54" s="18" t="s">
+    <row r="56" spans="1:10" ht="137" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="27"/>
+      <c r="B56" s="18" t="s">
         <v>424</v>
       </c>
-      <c r="C54" s="18" t="s">
+      <c r="C56" s="18" t="s">
         <v>425</v>
       </c>
-      <c r="D54" s="18" t="s">
+      <c r="D56" s="18" t="s">
         <v>426</v>
       </c>
-      <c r="E54" s="18" t="s">
+      <c r="E56" s="18" t="s">
         <v>427</v>
       </c>
-      <c r="F54" s="18" t="s">
+      <c r="F56" s="18" t="s">
         <v>428</v>
       </c>
-      <c r="G54" s="18" t="s">
+      <c r="G56" s="18" t="s">
         <v>429</v>
       </c>
-      <c r="H54" s="18" t="s">
+      <c r="H56" s="18" t="s">
         <v>430</v>
       </c>
-      <c r="I54" s="18" t="s">
+      <c r="I56" s="18" t="s">
         <v>431</v>
       </c>
-      <c r="J54" s="19" t="s">
+      <c r="J56" s="19" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="176" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="20" t="s">
+    <row r="65" spans="1:10" ht="176" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="20" t="s">
         <v>433</v>
       </c>
-      <c r="B63" s="21" t="s">
+      <c r="B65" s="21" t="s">
         <v>434</v>
       </c>
-      <c r="C63" s="21" t="s">
+      <c r="C65" s="21" t="s">
         <v>435</v>
       </c>
-      <c r="D63" s="21" t="s">
+      <c r="D65" s="21" t="s">
         <v>436</v>
       </c>
-      <c r="E63" s="21" t="s">
+      <c r="E65" s="21" t="s">
         <v>437</v>
       </c>
-      <c r="F63" s="21" t="s">
+      <c r="F65" s="21" t="s">
         <v>438</v>
       </c>
-      <c r="G63" s="21" t="s">
+      <c r="G65" s="21" t="s">
         <v>439</v>
       </c>
-      <c r="H63" s="21" t="s">
+      <c r="H65" s="21" t="s">
         <v>440</v>
       </c>
-      <c r="I63" s="21" t="s">
+      <c r="I65" s="21" t="s">
         <v>441</v>
       </c>
-      <c r="J63" s="21"/>
+      <c r="J65" s="21"/>
     </row>
-    <row r="64" spans="1:10" ht="140" x14ac:dyDescent="0.25">
-      <c r="A64" s="20" t="s">
+    <row r="66" spans="1:10" ht="140" x14ac:dyDescent="0.25">
+      <c r="A66" s="20" t="s">
         <v>442</v>
       </c>
-      <c r="B64" s="21" t="s">
+      <c r="B66" s="21" t="s">
         <v>443</v>
       </c>
-      <c r="C64" s="21" t="s">
+      <c r="C66" s="21" t="s">
         <v>444</v>
       </c>
-      <c r="D64" s="21" t="s">
+      <c r="D66" s="21" t="s">
         <v>445</v>
       </c>
-      <c r="E64" s="21" t="s">
+      <c r="E66" s="21" t="s">
         <v>446</v>
       </c>
-      <c r="F64" s="21" t="s">
+      <c r="F66" s="21" t="s">
         <v>447</v>
       </c>
-      <c r="G64" s="21" t="s">
+      <c r="G66" s="21" t="s">
         <v>448</v>
       </c>
-      <c r="H64" s="21" t="s">
+      <c r="H66" s="21" t="s">
         <v>449</v>
       </c>
-      <c r="I64" s="21" t="s">
+      <c r="I66" s="21" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B68" s="19"/>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B70" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="26">
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
@@ -47649,24 +47900,25 @@
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A20:A21"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A27"/>
     <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A19:A20"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A36:A37"/>
     <mergeCell ref="A48:A49"/>
     <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A55:A56"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A46:A47"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Add random forest regression
</commit_message>
<xml_diff>
--- a/Performance Record.xlsx
+++ b/Performance Record.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="567">
   <si>
     <r>
       <rPr>
@@ -41077,12 +41077,448 @@
       <t>PLA</t>
     </r>
   </si>
+  <si>
+    <t>TRAIN:
+minimumPrice: 44.4344444444
+maximumPrice: 115.915925926
+randomPrice: 68.4391315136
+avgPredPrice: 44.4344444444
+Performance: 35.07%
+Max Perfor: 35.07%
+Normalized perfor: 100.0%</t>
+  </si>
+  <si>
+    <t>TRAIN:
+minimumPrice: 49.6566666667
+maximumPrice: 129.656666667
+randomPrice: 77.4751720047
+avgPredPrice: 49.6566666667
+Performance: 35.91%
+Max Perfor: 35.91%
+Normalized perfor: 100.0%</t>
+  </si>
+  <si>
+    <t>TRAIN:
+minimumPrice: 48.2691891892
+maximumPrice: 141.252972973
+randomPrice: 75.0340018399
+avgPredPrice: 48.5286486486
+Performance: 35.32%
+Max Perfor: 35.67%
+Normalized perfor: 99.03%</t>
+  </si>
+  <si>
+    <t>TRAIN:
+minimumPrice: 47.0833333333
+maximumPrice: 149.972222222
+randomPrice: 73.9964736451
+avgPredPrice: 47.0833333333
+Performance: 36.37%
+Max Perfor: 36.37%
+Normalized perfor: 100.0%</t>
+  </si>
+  <si>
+    <t>TRAIN:
+minimumPrice: 68.982
+maximumPrice: 174.402
+randomPrice: 105.280932384
+avgPredPrice: 68.982
+Performance: 34.48%
+Max Perfor: 34.48%
+Normalized perfor: 100.0%</t>
+  </si>
+  <si>
+    <t>TRAIN:
+minimumPrice: 63.1279459459
+maximumPrice: 160.91172973
+randomPrice: 97.1720369004
+avgPredPrice: 63.1279459459
+Performance: 35.03%
+Max Perfor: 35.03%
+Normalized perfor: 100.0%</t>
+  </si>
+  <si>
+    <t>Average Performance: 35.1%
+Average Normalized Performance: 99.88%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 32.370952381
+maximumPrice: 126.656666667
+randomPrice: 55.4820634921
+avgPredPrice: 49.99
+Performance: 9.9%
+Max Perfor: 41.66%
+Normalized perfor: 23.76%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 29.3775238095
+maximumPrice: 168.95847619
+randomPrice: 57.8067301587
+avgPredPrice: 51.0156190476
+Performance: 11.75%
+Max Perfor: 49.18%
+Normalized perfor: 23.89%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 11.3788888889
+maximumPrice: 93.6011111111
+randomPrice: 23.152037037
+avgPredPrice: 16.6566666667
+Performance: 28.06%
+Max Perfor: 50.85%
+Normalized perfor: 55.17%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 16.5284615385
+maximumPrice: 90.5669230769
+randomPrice: 33.3727319588
+avgPredPrice: 33.6438461538
+Performance: -0.81%
+Max Perfor: 50.47%
+Normalized perfor: -1.61%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 18.6184615385
+maximumPrice: 101.233846154
+randomPrice: 35.3032044199
+avgPredPrice: 43.0338461538
+Performance: -21.9%
+Max Perfor: 47.26%
+Normalized perfor: -46.33%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 14.6111111111
+maximumPrice: 198.361111111
+randomPrice: 41.1180555556
+avgPredPrice: 43.9861111111
+Performance: -6.98%
+Max Perfor: 64.47%
+Normalized perfor: -10.82%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 21.5127692308
+maximumPrice: 154.505076923
+randomPrice: 56.3433402062
+avgPredPrice: 44.2204615385
+Performance: 21.52%
+Max Perfor: 61.82%
+Normalized perfor: 34.81%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 25.8050769231
+maximumPrice: 208.020461538
+randomPrice: 60.2546519337
+avgPredPrice: 79.182
+Performance: -31.41%
+Max Perfor: 57.17%
+Normalized perfor: -54.94%</t>
+  </si>
+  <si>
+    <t>Average Performance: 1.27%
+Average Normalized Performance: 2.99%</t>
+  </si>
+  <si>
+    <t>Uniform Blending Classification
+logistic regression, AdaBoost with Decision Tree, KNN, Decision Tree, Neural Network, Random Forest</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 32.370952381
+maximumPrice: 126.656666667
+randomPrice: 55.4820634921
+avgPredPrice: 41.8947619048
+Performance: 24.49%
+Max Perfor: 41.66%
+Normalized perfor: 58.79%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 11.3788888889
+maximumPrice: 93.6011111111
+randomPrice: 23.152037037
+avgPredPrice: 13.4622222222
+Performance: 41.85%
+Max Perfor: 50.85%
+Normalized perfor: 82.3%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 16.5284615385
+maximumPrice: 90.5669230769
+randomPrice: 33.3727319588
+avgPredPrice: 22.8746153846
+Performance: 31.46%
+Max Perfor: 50.47%
+Normalized perfor: 62.32%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 18.6184615385
+maximumPrice: 101.233846154
+randomPrice: 35.3032044199
+avgPredPrice: 32.5107692308
+Performance: 7.91%
+Max Perfor: 47.26%
+Normalized perfor: 16.74%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 14.6111111111
+maximumPrice: 198.361111111
+randomPrice: 41.1180555556
+avgPredPrice: 19.75
+Performance: 51.97%
+Max Perfor: 64.47%
+Normalized perfor: 80.61%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 21.5127692308
+maximumPrice: 154.505076923
+randomPrice: 56.3433402062
+avgPredPrice: 37.5743076923
+Performance: 33.31%
+Max Perfor: 61.82%
+Normalized perfor: 53.89%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 25.8050769231
+maximumPrice: 208.020461538
+randomPrice: 60.2546519337
+avgPredPrice: 53.6358461538
+Performance: 10.98%
+Max Perfor: 57.17%
+Normalized perfor: 19.21%</t>
+  </si>
+  <si>
+    <t>Average Performance: 29.02%
+Average Normalized Performance: 54.41%</t>
+  </si>
+  <si>
+    <t>TRAIN:
+minimumPrice: 44.4344444444
+maximumPrice: 115.915925926
+randomPrice: 68.4391315136
+avgPredPrice: 45.1751851852
+Performance: 33.99%
+Max Perfor: 35.07%
+Normalized perfor: 96.91%</t>
+  </si>
+  <si>
+    <t>TRAIN:
+minimumPrice: 38.9605925926
+maximumPrice: 126.782814815
+randomPrice: 67.4260645161
+avgPredPrice: 40.9754074074
+Performance: 39.23%
+Max Perfor: 42.22%
+Normalized perfor: 92.92%</t>
+  </si>
+  <si>
+    <t>TRAIN:
+minimumPrice: 68.6566666667
+maximumPrice: 144.212222222
+randomPrice: 93.2808545727
+avgPredPrice: 74.99
+Performance: 19.61%
+Max Perfor: 26.4%
+Normalized perfor: 74.28%</t>
+  </si>
+  <si>
+    <t>TRAIN:
+minimumPrice: 48.2691891892
+maximumPrice: 141.252972973
+randomPrice: 75.0340018399
+avgPredPrice: 53.3286486486
+Performance: 28.93%
+Max Perfor: 35.67%
+Normalized perfor: 81.1%</t>
+  </si>
+  <si>
+    <t>TRAIN:
+minimumPrice: 47.0833333333
+maximumPrice: 149.972222222
+randomPrice: 73.9964736451
+avgPredPrice: 47.8055555556
+Performance: 35.39%
+Max Perfor: 36.37%
+Normalized perfor: 97.32%</t>
+  </si>
+  <si>
+    <t>TRAIN:
+minimumPrice: 63.1279459459
+maximumPrice: 160.91172973
+randomPrice: 97.1720369004
+avgPredPrice: 67.7982162162
+Performance: 30.23%
+Max Perfor: 35.03%
+Normalized perfor: 86.28%</t>
+  </si>
+  <si>
+    <t>Average Performance: 31.43%
+Average Normalized Performance: 88.87%</t>
+  </si>
+  <si>
+    <t>Random Forest Classification
+max_features='sqrt', n_estimators=32, max_depth=58</t>
+  </si>
+  <si>
+    <t>Random Forest Regression
+max_features=None, n_estimators=21, max_depth=55</t>
+  </si>
+  <si>
+    <t>TRAIN:
+minimumPrice: 68.6566666667
+maximumPrice: 144.212222222
+randomPrice: 93.2808545727
+avgPredPrice: 70.3233333333
+Performance: 24.61%
+Max Perfor: 26.4%
+Normalized perfor: 93.23%</t>
+  </si>
+  <si>
+    <t>TRAIN:
+minimumPrice: 49.6566666667
+maximumPrice: 129.656666667
+randomPrice: 77.4751720047
+avgPredPrice: 51.8233333333
+Performance: 33.11%
+Max Perfor: 35.91%
+Normalized perfor: 92.21%</t>
+  </si>
+  <si>
+    <t>TRAIN:
+minimumPrice: 48.2691891892
+maximumPrice: 141.252972973
+randomPrice: 75.0340018399
+avgPredPrice: 50.2151351351
+Performance: 33.08%
+Max Perfor: 35.67%
+Normalized perfor: 92.73%</t>
+  </si>
+  <si>
+    <t>TRAIN:
+minimumPrice: 47.0833333333
+maximumPrice: 149.972222222
+randomPrice: 73.9964736451
+avgPredPrice: 49.9722222222
+Performance: 32.47%
+Max Perfor: 36.37%
+Normalized perfor: 89.27%</t>
+  </si>
+  <si>
+    <t>TRAIN:
+minimumPrice: 68.982
+maximumPrice: 174.402
+randomPrice: 105.280932384
+avgPredPrice: 69.162
+Performance: 34.31%
+Max Perfor: 34.48%
+Normalized perfor: 99.5%</t>
+  </si>
+  <si>
+    <t>TRAIN:
+minimumPrice: 63.1279459459
+maximumPrice: 160.91172973
+randomPrice: 97.1720369004
+avgPredPrice: 64.2955135135
+Performance: 33.83%
+Max Perfor: 35.03%
+Normalized perfor: 96.57%</t>
+  </si>
+  <si>
+    <t>Average Performance: 33.65%
+Average Normalized Performance: 95.6%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 29.3775238095
+maximumPrice: 168.95847619
+randomPrice: 57.8067301587
+avgPredPrice: 36.0822857143
+Performance: 37.58%
+Max Perfor: 49.18%
+Normalized perfor: 76.42%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 11.3788888889
+maximumPrice: 93.6011111111
+randomPrice: 23.152037037
+avgPredPrice: 17.49
+Performance: 24.46%
+Max Perfor: 50.85%
+Normalized perfor: 48.09%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 16.5284615385
+maximumPrice: 90.5669230769
+randomPrice: 33.3727319588
+avgPredPrice: 27.1053846154
+Performance: 18.78%
+Max Perfor: 50.47%
+Normalized perfor: 37.21%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 18.6184615385
+maximumPrice: 101.233846154
+randomPrice: 35.3032044199
+avgPredPrice: 26.4646153846
+Performance: 25.04%
+Max Perfor: 47.26%
+Normalized perfor: 52.97%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 14.6111111111
+maximumPrice: 198.361111111
+randomPrice: 41.1180555556
+avgPredPrice: 22.6666666667
+Performance: 44.87%
+Max Perfor: 64.47%
+Normalized perfor: 69.61%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 21.5127692308
+maximumPrice: 154.505076923
+randomPrice: 56.3433402062
+avgPredPrice: 37.2281538462
+Performance: 33.93%
+Max Perfor: 61.82%
+Normalized perfor: 54.88%</t>
+  </si>
+  <si>
+    <t>TEST:
+minimumPrice: 25.8050769231
+maximumPrice: 208.020461538
+randomPrice: 60.2546519337
+avgPredPrice: 57.5127692308
+Performance: 4.55%
+Max Perfor: 57.17%
+Normalized perfor: 7.96%</t>
+  </si>
+  <si>
+    <t>Average Performance: 25.53%
+Average Normalized Performance: 47.91%</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="70" x14ac:knownFonts="1">
+  <fonts count="72" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -41493,6 +41929,18 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -41539,7 +41987,7 @@
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -41614,6 +42062,9 @@
     <xf numFmtId="0" fontId="66" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -41655,22 +42106,34 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -41963,10 +42426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K76"/>
+  <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="82" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="82" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -42033,7 +42496,7 @@
       <c r="K2" s="22"/>
     </row>
     <row r="3" spans="1:11" ht="151" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="42" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -42064,7 +42527,7 @@
       <c r="K3" s="22"/>
     </row>
     <row r="4" spans="1:11" ht="154" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="6" t="s">
         <v>21</v>
       </c>
@@ -42095,7 +42558,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="161" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="50" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -42128,7 +42591,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="159" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="1" t="s">
         <v>40</v>
       </c>
@@ -42157,7 +42620,7 @@
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="31" t="s">
         <v>48</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -42188,7 +42651,7 @@
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" ht="188" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="31"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="8" t="s">
         <v>57</v>
       </c>
@@ -42219,7 +42682,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="160" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="33" t="s">
         <v>66</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -42250,7 +42713,7 @@
       <c r="K9" s="23"/>
     </row>
     <row r="10" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="5" t="s">
         <v>75</v>
       </c>
@@ -42279,7 +42742,7 @@
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="33" t="s">
         <v>83</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -42310,7 +42773,7 @@
       <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="5" t="s">
         <v>92</v>
       </c>
@@ -42339,7 +42802,7 @@
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="33" t="s">
         <v>100</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -42370,7 +42833,7 @@
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="5" t="s">
         <v>108</v>
       </c>
@@ -42399,7 +42862,7 @@
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="34" t="s">
         <v>116</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -42430,7 +42893,7 @@
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="5" t="s">
         <v>125</v>
       </c>
@@ -42461,7 +42924,7 @@
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="42" t="s">
         <v>458</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -42494,7 +42957,7 @@
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="37"/>
+      <c r="A18" s="38"/>
       <c r="B18" s="5" t="s">
         <v>448</v>
       </c>
@@ -42525,7 +42988,7 @@
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="44" t="s">
         <v>485</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -42558,7 +43021,7 @@
       <c r="K19" s="1"/>
     </row>
     <row r="20" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="45"/>
       <c r="B20" s="5" t="s">
         <v>476</v>
       </c>
@@ -42589,7 +43052,7 @@
       <c r="K20" s="1"/>
     </row>
     <row r="21" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="45" t="s">
+      <c r="A21" s="44" t="s">
         <v>489</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -42624,7 +43087,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="45"/>
+      <c r="A22" s="44"/>
       <c r="B22" s="5" t="s">
         <v>490</v>
       </c>
@@ -42655,7 +43118,7 @@
       <c r="K22" s="1"/>
     </row>
     <row r="23" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="44" t="s">
         <v>517</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -42672,7 +43135,7 @@
       <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="48"/>
+      <c r="A24" s="45"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -42685,1191 +43148,1381 @@
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="47" t="s">
-        <v>515</v>
+      <c r="A25" s="48" t="s">
+        <v>534</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>457</v>
+        <v>543</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>459</v>
+        <v>544</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>508</v>
+        <v>545</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>509</v>
+        <v>470</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>510</v>
+        <v>546</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>511</v>
+        <v>547</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>512</v>
+        <v>473</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>513</v>
+        <v>548</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>514</v>
+        <v>549</v>
       </c>
       <c r="K25" s="1"/>
     </row>
     <row r="26" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
+      <c r="A26" s="49"/>
       <c r="B26" s="5" t="s">
-        <v>448</v>
+        <v>535</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>449</v>
+        <v>491</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>451</v>
+        <v>536</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>537</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>452</v>
+        <v>538</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>453</v>
+        <v>539</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>454</v>
+        <v>540</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>455</v>
+        <v>541</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>456</v>
+        <v>542</v>
       </c>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
+    <row r="27" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="46" t="s">
+        <v>515</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>509</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>514</v>
+      </c>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:11" ht="154" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="41" t="s">
-        <v>135</v>
-      </c>
+    <row r="28" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="46"/>
       <c r="B28" s="5" t="s">
-        <v>136</v>
+        <v>448</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>137</v>
+        <v>449</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>139</v>
+        <v>450</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>451</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>140</v>
+        <v>452</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>141</v>
+        <v>453</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>142</v>
+        <v>454</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="J28" s="5"/>
+        <v>455</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>456</v>
+      </c>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11" ht="167" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="31"/>
-      <c r="B29" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="J29" s="6"/>
-      <c r="K29" s="1" t="s">
-        <v>152</v>
-      </c>
+    <row r="29" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="47" t="s">
+        <v>550</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>518</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>500</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="E29" s="26" t="s">
+        <v>519</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>520</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>521</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" ht="169" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="42" t="s">
-        <v>153</v>
-      </c>
+    <row r="30" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="47"/>
       <c r="B30" s="5" t="s">
-        <v>154</v>
+        <v>525</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>155</v>
+        <v>526</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>159</v>
+        <v>527</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>528</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>529</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>530</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>160</v>
+        <v>531</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="J30" s="5"/>
+        <v>532</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>533</v>
+      </c>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" ht="133" x14ac:dyDescent="0.25">
-      <c r="A31" s="37"/>
-      <c r="B31" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="F31" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="G31" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="H31" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="I31" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="J31" s="13"/>
-      <c r="K31" s="1" t="s">
-        <v>170</v>
-      </c>
+    <row r="31" spans="1:11" ht="158" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="154" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="42" t="s">
-        <v>171</v>
-      </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
+        <v>135</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="J32" s="5"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" ht="133" x14ac:dyDescent="0.25">
-      <c r="A33" s="37"/>
-      <c r="B33" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="J33" s="5"/>
-      <c r="K33" s="20"/>
+    <row r="33" spans="1:11" ht="167" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="32"/>
+      <c r="B33" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="J33" s="6"/>
+      <c r="K33" s="1" t="s">
+        <v>152</v>
+      </c>
     </row>
-    <row r="34" spans="1:11" ht="152" x14ac:dyDescent="0.25">
-      <c r="A34" s="36" t="s">
-        <v>180</v>
+    <row r="34" spans="1:11" ht="169" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="43" t="s">
+        <v>153</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>181</v>
+        <v>154</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>182</v>
+        <v>155</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>183</v>
+        <v>156</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>187</v>
+        <v>160</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>188</v>
+        <v>161</v>
       </c>
       <c r="J34" s="5"/>
-      <c r="K34" s="20"/>
+      <c r="K34" s="1"/>
     </row>
     <row r="35" spans="1:11" ht="133" x14ac:dyDescent="0.25">
-      <c r="A35" s="37"/>
-      <c r="B35" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="J35" s="5"/>
-      <c r="K35" s="20"/>
+      <c r="A35" s="38"/>
+      <c r="B35" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="J35" s="13"/>
+      <c r="K35" s="1" t="s">
+        <v>170</v>
+      </c>
     </row>
-    <row r="36" spans="1:11" ht="152" x14ac:dyDescent="0.25">
-      <c r="A36" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="J36" s="5"/>
-      <c r="K36" s="20"/>
+    <row r="36" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A36" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" ht="182" x14ac:dyDescent="0.3">
-      <c r="A37" s="31"/>
-      <c r="B37" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="H37" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I37" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="J37" s="8"/>
+    <row r="37" spans="1:11" ht="133" x14ac:dyDescent="0.25">
+      <c r="A37" s="38"/>
+      <c r="B37" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="J37" s="5"/>
       <c r="K37" s="20"/>
     </row>
     <row r="38" spans="1:11" ht="152" x14ac:dyDescent="0.25">
-      <c r="A38" s="36" t="s">
-        <v>214</v>
+      <c r="A38" s="37" t="s">
+        <v>180</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>215</v>
+        <v>181</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>216</v>
+        <v>182</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>217</v>
+        <v>183</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>218</v>
+        <v>184</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>219</v>
+        <v>185</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>220</v>
+        <v>186</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>221</v>
+        <v>187</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>222</v>
+        <v>188</v>
       </c>
       <c r="J38" s="5"/>
       <c r="K38" s="20"/>
     </row>
     <row r="39" spans="1:11" ht="133" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
-      <c r="B39" s="5" t="s">
-        <v>223</v>
+      <c r="A39" s="38"/>
+      <c r="B39" s="10" t="s">
+        <v>189</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>224</v>
+        <v>190</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>226</v>
+        <v>192</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>227</v>
+        <v>193</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>228</v>
+        <v>194</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>229</v>
+        <v>195</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>230</v>
+        <v>196</v>
       </c>
       <c r="J39" s="5"/>
       <c r="K39" s="20"/>
     </row>
     <row r="40" spans="1:11" ht="152" x14ac:dyDescent="0.25">
       <c r="A40" s="39" t="s">
-        <v>231</v>
+        <v>197</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>232</v>
+        <v>198</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>233</v>
+        <v>199</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>234</v>
+        <v>200</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>235</v>
+        <v>201</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>236</v>
+        <v>202</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>237</v>
+        <v>203</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>238</v>
+        <v>204</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>239</v>
+        <v>205</v>
       </c>
       <c r="J40" s="5"/>
       <c r="K40" s="20"/>
     </row>
     <row r="41" spans="1:11" ht="182" x14ac:dyDescent="0.3">
-      <c r="A41" s="40"/>
+      <c r="A41" s="32"/>
       <c r="B41" s="8" t="s">
-        <v>240</v>
+        <v>206</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>241</v>
+        <v>207</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>242</v>
+        <v>208</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>243</v>
+        <v>209</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>244</v>
+        <v>210</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>245</v>
+        <v>211</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>246</v>
+        <v>212</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>247</v>
+        <v>213</v>
       </c>
       <c r="J41" s="8"/>
       <c r="K41" s="20"/>
     </row>
     <row r="42" spans="1:11" ht="152" x14ac:dyDescent="0.25">
-      <c r="A42" s="36" t="s">
-        <v>248</v>
+      <c r="A42" s="37" t="s">
+        <v>214</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>249</v>
+        <v>215</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>250</v>
+        <v>216</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>251</v>
+        <v>217</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>252</v>
+        <v>218</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>253</v>
+        <v>219</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>254</v>
+        <v>220</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>255</v>
+        <v>221</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
       <c r="J42" s="5"/>
       <c r="K42" s="20"/>
     </row>
     <row r="43" spans="1:11" ht="133" x14ac:dyDescent="0.25">
-      <c r="A43" s="31"/>
+      <c r="A43" s="32"/>
       <c r="B43" s="5" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>259</v>
+        <v>225</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>260</v>
+        <v>226</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>261</v>
+        <v>227</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>262</v>
+        <v>228</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="I43" s="10" t="s">
-        <v>264</v>
-      </c>
-      <c r="J43" s="10"/>
+        <v>229</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="J43" s="5"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" ht="162" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="30" t="s">
-        <v>265</v>
+    <row r="44" spans="1:11" ht="152" x14ac:dyDescent="0.25">
+      <c r="A44" s="40" t="s">
+        <v>231</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>266</v>
+        <v>232</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>267</v>
+        <v>233</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>268</v>
+        <v>234</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>269</v>
+        <v>235</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>270</v>
+        <v>236</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>271</v>
+        <v>237</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>272</v>
+        <v>238</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>273</v>
+        <v>239</v>
       </c>
       <c r="J44" s="5"/>
       <c r="K44" s="20"/>
     </row>
     <row r="45" spans="1:11" ht="182" x14ac:dyDescent="0.3">
-      <c r="A45" s="31"/>
+      <c r="A45" s="41"/>
       <c r="B45" s="8" t="s">
-        <v>274</v>
+        <v>240</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>275</v>
+        <v>241</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>277</v>
+        <v>243</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>278</v>
+        <v>244</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>279</v>
+        <v>245</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>280</v>
+        <v>246</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>281</v>
+        <v>247</v>
       </c>
       <c r="J45" s="8"/>
-      <c r="K45" s="23" t="s">
-        <v>65</v>
-      </c>
+      <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" ht="163" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="32" t="s">
-        <v>282</v>
+    <row r="46" spans="1:11" ht="152" x14ac:dyDescent="0.25">
+      <c r="A46" s="37" t="s">
+        <v>248</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>283</v>
+        <v>249</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>284</v>
+        <v>250</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>285</v>
+        <v>251</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>286</v>
+        <v>252</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>287</v>
+        <v>253</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>288</v>
+        <v>254</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>289</v>
+        <v>255</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>290</v>
+        <v>256</v>
       </c>
       <c r="J46" s="5"/>
-      <c r="K46" s="23"/>
+      <c r="K46" s="20"/>
     </row>
     <row r="47" spans="1:11" ht="133" x14ac:dyDescent="0.25">
-      <c r="A47" s="31"/>
+      <c r="A47" s="32"/>
       <c r="B47" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="I47" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="J47" s="10"/>
+      <c r="K47" s="20"/>
+    </row>
+    <row r="48" spans="1:11" ht="162" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="J48" s="5"/>
+      <c r="K48" s="20"/>
+    </row>
+    <row r="49" spans="1:11" ht="182" x14ac:dyDescent="0.3">
+      <c r="A49" s="32"/>
+      <c r="B49" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H49" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I49" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="J49" s="8"/>
+      <c r="K49" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="163" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="33" t="s">
+        <v>282</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="J50" s="5"/>
+      <c r="K50" s="23"/>
+    </row>
+    <row r="51" spans="1:11" ht="133" x14ac:dyDescent="0.25">
+      <c r="A51" s="32"/>
+      <c r="B51" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C51" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D51" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E51" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="F47" s="5" t="s">
+      <c r="F51" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="G47" s="5" t="s">
+      <c r="G51" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="H47" s="5" t="s">
+      <c r="H51" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="I47" s="5" t="s">
+      <c r="I51" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="J47" s="5" t="s">
+      <c r="J51" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="K47" s="22"/>
+      <c r="K51" s="22"/>
     </row>
-    <row r="48" spans="1:11" ht="146" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="32" t="s">
+    <row r="52" spans="1:11" ht="146" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="33" t="s">
         <v>300</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B52" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C52" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D52" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="E52" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="F48" s="5" t="s">
+      <c r="F52" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="G48" s="5" t="s">
+      <c r="G52" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="H48" s="5" t="s">
+      <c r="H52" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="I48" s="5" t="s">
+      <c r="I52" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="J48" s="5"/>
-      <c r="K48" s="22"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="22"/>
     </row>
-    <row r="49" spans="1:11" ht="149" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="31"/>
-      <c r="B49" s="5" t="s">
+    <row r="53" spans="1:11" ht="149" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="32"/>
+      <c r="B53" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C53" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D53" s="5" t="s">
         <v>311</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="E53" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="F53" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="G49" s="5" t="s">
+      <c r="G53" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="H49" s="5" t="s">
+      <c r="H53" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="I49" s="5" t="s">
+      <c r="I53" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="J49" s="5" t="s">
+      <c r="J53" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="K49" s="22"/>
+      <c r="K53" s="22"/>
     </row>
-    <row r="50" spans="1:11" ht="129" x14ac:dyDescent="0.25">
-      <c r="A50" s="33" t="s">
+    <row r="54" spans="1:11" ht="129" x14ac:dyDescent="0.25">
+      <c r="A54" s="34" t="s">
         <v>318</v>
       </c>
-      <c r="B50" s="15" t="s">
+      <c r="B54" s="15" t="s">
         <v>319</v>
       </c>
-      <c r="C50" s="15" t="s">
+      <c r="C54" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="D50" s="15" t="s">
+      <c r="D54" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="E50" s="15" t="s">
+      <c r="E54" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="F50" s="15" t="s">
+      <c r="F54" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G50" s="15" t="s">
+      <c r="G54" s="15" t="s">
         <v>324</v>
       </c>
-      <c r="H50" s="15" t="s">
+      <c r="H54" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="I50" s="15" t="s">
+      <c r="I54" s="15" t="s">
         <v>326</v>
       </c>
-      <c r="J50" s="19" t="s">
+      <c r="J54" s="19" t="s">
         <v>327</v>
       </c>
-      <c r="K50" s="13" t="s">
+      <c r="K54" s="13" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="131" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="31"/>
-      <c r="B51" s="15" t="s">
+    <row r="55" spans="1:11" ht="131" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="32"/>
+      <c r="B55" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="C51" s="15" t="s">
+      <c r="C55" s="15" t="s">
         <v>329</v>
       </c>
-      <c r="D51" s="15" t="s">
+      <c r="D55" s="15" t="s">
         <v>330</v>
       </c>
-      <c r="E51" s="15" t="s">
+      <c r="E55" s="15" t="s">
         <v>331</v>
       </c>
-      <c r="F51" s="15" t="s">
+      <c r="F55" s="15" t="s">
         <v>332</v>
       </c>
-      <c r="G51" s="15" t="s">
+      <c r="G55" s="15" t="s">
         <v>333</v>
       </c>
-      <c r="H51" s="15" t="s">
+      <c r="H55" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="I51" s="15" t="s">
+      <c r="I55" s="15" t="s">
         <v>335</v>
       </c>
-      <c r="J51" s="19" t="s">
+      <c r="J55" s="19" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="128" x14ac:dyDescent="0.2">
-      <c r="A52" s="34" t="s">
+    <row r="56" spans="1:11" ht="128" x14ac:dyDescent="0.2">
+      <c r="A56" s="35" t="s">
         <v>337</v>
       </c>
-      <c r="B52" s="15" t="s">
+      <c r="B56" s="15" t="s">
         <v>338</v>
       </c>
-      <c r="C52" s="15" t="s">
+      <c r="C56" s="15" t="s">
         <v>339</v>
       </c>
-      <c r="D52" s="15" t="s">
+      <c r="D56" s="15" t="s">
         <v>340</v>
       </c>
-      <c r="E52" s="15" t="s">
+      <c r="E56" s="15" t="s">
         <v>341</v>
       </c>
-      <c r="F52" s="15" t="s">
+      <c r="F56" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="G52" s="15" t="s">
+      <c r="G56" s="15" t="s">
         <v>343</v>
       </c>
-      <c r="H52" s="16" t="s">
+      <c r="H56" s="16" t="s">
         <v>344</v>
       </c>
-      <c r="I52" s="15" t="s">
+      <c r="I56" s="15" t="s">
         <v>345</v>
       </c>
-      <c r="J52" s="19" t="s">
+      <c r="J56" s="19" t="s">
         <v>346</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="144" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="35"/>
-      <c r="B53" s="17" t="s">
-        <v>347</v>
-      </c>
-      <c r="C53" s="17" t="s">
-        <v>348</v>
-      </c>
-      <c r="D53" s="17" t="s">
-        <v>349</v>
-      </c>
-      <c r="E53" s="17" t="s">
-        <v>350</v>
-      </c>
-      <c r="F53" s="17" t="s">
-        <v>351</v>
-      </c>
-      <c r="G53" s="17" t="s">
-        <v>352</v>
-      </c>
-      <c r="H53" s="17" t="s">
-        <v>353</v>
-      </c>
-      <c r="I53" s="17" t="s">
-        <v>354</v>
-      </c>
-      <c r="J53" s="24" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" ht="144" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="28" t="s">
-        <v>486</v>
-      </c>
-      <c r="B54" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="C54" s="18" t="s">
-        <v>357</v>
-      </c>
-      <c r="D54" s="18" t="s">
-        <v>358</v>
-      </c>
-      <c r="E54" s="18" t="s">
-        <v>359</v>
-      </c>
-      <c r="F54" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="G54" s="18" t="s">
-        <v>361</v>
-      </c>
-      <c r="H54" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="I54" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="J54" s="21" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="144" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="28"/>
-      <c r="B55" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="C55" s="18" t="s">
-        <v>366</v>
-      </c>
-      <c r="D55" s="18" t="s">
-        <v>367</v>
-      </c>
-      <c r="E55" s="18" t="s">
-        <v>368</v>
-      </c>
-      <c r="F55" s="18" t="s">
-        <v>369</v>
-      </c>
-      <c r="G55" s="18" t="s">
-        <v>370</v>
-      </c>
-      <c r="H55" s="18" t="s">
-        <v>371</v>
-      </c>
-      <c r="I55" s="18" t="s">
-        <v>372</v>
-      </c>
-      <c r="J55" s="21" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="144" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="28" t="s">
-        <v>487</v>
-      </c>
-      <c r="B56" s="18" t="s">
-        <v>374</v>
-      </c>
-      <c r="C56" s="18" t="s">
-        <v>375</v>
-      </c>
-      <c r="D56" s="18" t="s">
-        <v>376</v>
-      </c>
-      <c r="E56" s="18" t="s">
-        <v>377</v>
-      </c>
-      <c r="F56" s="18" t="s">
-        <v>378</v>
-      </c>
-      <c r="G56" s="18" t="s">
-        <v>379</v>
-      </c>
-      <c r="H56" s="18" t="s">
-        <v>380</v>
-      </c>
-      <c r="I56" s="18" t="s">
-        <v>381</v>
-      </c>
-      <c r="J56" s="21" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="144" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="28"/>
-      <c r="B57" s="18" t="s">
-        <v>383</v>
-      </c>
-      <c r="C57" s="18" t="s">
-        <v>384</v>
-      </c>
-      <c r="D57" s="18" t="s">
-        <v>385</v>
-      </c>
-      <c r="E57" s="18" t="s">
-        <v>386</v>
-      </c>
-      <c r="F57" s="18" t="s">
-        <v>387</v>
-      </c>
-      <c r="G57" s="18" t="s">
-        <v>388</v>
-      </c>
-      <c r="H57" s="18" t="s">
-        <v>389</v>
-      </c>
-      <c r="I57" s="18" t="s">
-        <v>390</v>
-      </c>
-      <c r="J57" s="21" t="s">
-        <v>391</v>
+      <c r="A57" s="36"/>
+      <c r="B57" s="17" t="s">
+        <v>347</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>348</v>
+      </c>
+      <c r="D57" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="E57" s="17" t="s">
+        <v>350</v>
+      </c>
+      <c r="F57" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="G57" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="H57" s="17" t="s">
+        <v>353</v>
+      </c>
+      <c r="I57" s="17" t="s">
+        <v>354</v>
+      </c>
+      <c r="J57" s="24" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="144" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="28" t="s">
+      <c r="A58" s="29" t="s">
+        <v>486</v>
+      </c>
+      <c r="B58" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>358</v>
+      </c>
+      <c r="E58" s="18" t="s">
+        <v>359</v>
+      </c>
+      <c r="F58" s="18" t="s">
+        <v>360</v>
+      </c>
+      <c r="G58" s="18" t="s">
+        <v>361</v>
+      </c>
+      <c r="H58" s="18" t="s">
+        <v>362</v>
+      </c>
+      <c r="I58" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="J58" s="21" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="29"/>
+      <c r="B59" s="18" t="s">
+        <v>365</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="E59" s="18" t="s">
+        <v>368</v>
+      </c>
+      <c r="F59" s="18" t="s">
+        <v>369</v>
+      </c>
+      <c r="G59" s="18" t="s">
+        <v>370</v>
+      </c>
+      <c r="H59" s="18" t="s">
+        <v>371</v>
+      </c>
+      <c r="I59" s="18" t="s">
+        <v>372</v>
+      </c>
+      <c r="J59" s="21" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="29" t="s">
+        <v>487</v>
+      </c>
+      <c r="B60" s="18" t="s">
+        <v>374</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>375</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>376</v>
+      </c>
+      <c r="E60" s="18" t="s">
+        <v>377</v>
+      </c>
+      <c r="F60" s="18" t="s">
+        <v>378</v>
+      </c>
+      <c r="G60" s="18" t="s">
+        <v>379</v>
+      </c>
+      <c r="H60" s="18" t="s">
+        <v>380</v>
+      </c>
+      <c r="I60" s="18" t="s">
+        <v>381</v>
+      </c>
+      <c r="J60" s="21" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="29"/>
+      <c r="B61" s="18" t="s">
+        <v>383</v>
+      </c>
+      <c r="C61" s="18" t="s">
+        <v>384</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>385</v>
+      </c>
+      <c r="E61" s="18" t="s">
+        <v>386</v>
+      </c>
+      <c r="F61" s="18" t="s">
+        <v>387</v>
+      </c>
+      <c r="G61" s="18" t="s">
+        <v>388</v>
+      </c>
+      <c r="H61" s="18" t="s">
+        <v>389</v>
+      </c>
+      <c r="I61" s="18" t="s">
+        <v>390</v>
+      </c>
+      <c r="J61" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="29" t="s">
         <v>488</v>
       </c>
-      <c r="B58" s="18" t="s">
+      <c r="B62" s="18" t="s">
         <v>392</v>
       </c>
-      <c r="C58" s="18" t="s">
+      <c r="C62" s="18" t="s">
         <v>393</v>
       </c>
-      <c r="D58" s="18" t="s">
+      <c r="D62" s="18" t="s">
         <v>394</v>
       </c>
-      <c r="E58" s="18" t="s">
+      <c r="E62" s="28" t="s">
         <v>395</v>
       </c>
-      <c r="F58" s="18" t="s">
+      <c r="F62" s="18" t="s">
         <v>396</v>
       </c>
-      <c r="G58" s="18" t="s">
+      <c r="G62" s="18" t="s">
         <v>397</v>
       </c>
-      <c r="H58" s="18" t="s">
+      <c r="H62" s="18" t="s">
         <v>398</v>
       </c>
-      <c r="I58" s="18" t="s">
+      <c r="I62" s="18" t="s">
         <v>399</v>
       </c>
-      <c r="J58" s="21" t="s">
+      <c r="J62" s="21" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="128" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="28"/>
-      <c r="B59" s="18" t="s">
+    <row r="63" spans="1:11" ht="128" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="29"/>
+      <c r="B63" s="18" t="s">
         <v>401</v>
       </c>
-      <c r="C59" s="18" t="s">
+      <c r="C63" s="18" t="s">
         <v>402</v>
       </c>
-      <c r="D59" s="18" t="s">
+      <c r="D63" s="18" t="s">
         <v>403</v>
       </c>
-      <c r="E59" s="18" t="s">
+      <c r="E63" s="18" t="s">
         <v>404</v>
       </c>
-      <c r="F59" s="18" t="s">
+      <c r="F63" s="18" t="s">
         <v>405</v>
       </c>
-      <c r="G59" s="18" t="s">
+      <c r="G63" s="18" t="s">
         <v>406</v>
       </c>
-      <c r="H59" s="18" t="s">
+      <c r="H63" s="18" t="s">
         <v>407</v>
       </c>
-      <c r="I59" s="25" t="s">
+      <c r="I63" s="25" t="s">
         <v>408</v>
       </c>
-      <c r="J59" s="19" t="s">
+      <c r="J63" s="19" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="26" x14ac:dyDescent="0.3">
-      <c r="A60" s="11" t="s">
+    <row r="64" spans="1:11" ht="128" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="53" t="s">
+        <v>551</v>
+      </c>
+      <c r="B64" s="28" t="s">
+        <v>518</v>
+      </c>
+      <c r="C64" s="51">
+        <v>1</v>
+      </c>
+      <c r="D64" s="28" t="s">
+        <v>552</v>
+      </c>
+      <c r="E64" s="28" t="s">
+        <v>553</v>
+      </c>
+      <c r="F64" s="28" t="s">
+        <v>554</v>
+      </c>
+      <c r="G64" s="28" t="s">
+        <v>555</v>
+      </c>
+      <c r="H64" s="28" t="s">
+        <v>556</v>
+      </c>
+      <c r="I64" s="52" t="s">
+        <v>557</v>
+      </c>
+      <c r="J64" s="19" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="128" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="53"/>
+      <c r="B65" s="28" t="s">
+        <v>448</v>
+      </c>
+      <c r="C65" s="28" t="s">
+        <v>559</v>
+      </c>
+      <c r="D65" s="28" t="s">
+        <v>560</v>
+      </c>
+      <c r="E65" s="28" t="s">
+        <v>561</v>
+      </c>
+      <c r="F65" s="28" t="s">
+        <v>562</v>
+      </c>
+      <c r="G65" s="28" t="s">
+        <v>563</v>
+      </c>
+      <c r="H65" s="28" t="s">
+        <v>564</v>
+      </c>
+      <c r="I65" s="52" t="s">
+        <v>565</v>
+      </c>
+      <c r="J65" s="19" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="26" x14ac:dyDescent="0.3">
+      <c r="A66" s="11" t="s">
         <v>410</v>
       </c>
-      <c r="B60" s="19"/>
-      <c r="C60" s="19"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="19"/>
-      <c r="F60" s="19"/>
-      <c r="G60" s="19"/>
-      <c r="H60" s="19"/>
-      <c r="I60" s="19"/>
-      <c r="J60" s="19"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="19"/>
+      <c r="G66" s="19"/>
+      <c r="H66" s="19"/>
+      <c r="I66" s="19"/>
+      <c r="J66" s="19"/>
     </row>
-    <row r="61" spans="1:11" ht="128" x14ac:dyDescent="0.2">
-      <c r="A61" s="29" t="s">
+    <row r="67" spans="1:10" ht="128" x14ac:dyDescent="0.2">
+      <c r="A67" s="30" t="s">
         <v>411</v>
       </c>
-      <c r="B61" s="18" t="s">
+      <c r="B67" s="18" t="s">
         <v>412</v>
       </c>
-      <c r="C61" s="18" t="s">
+      <c r="C67" s="18" t="s">
         <v>413</v>
       </c>
-      <c r="D61" s="18" t="s">
+      <c r="D67" s="18" t="s">
         <v>414</v>
       </c>
-      <c r="E61" s="18" t="s">
+      <c r="E67" s="18" t="s">
         <v>415</v>
       </c>
-      <c r="F61" s="18" t="s">
+      <c r="F67" s="18" t="s">
         <v>416</v>
       </c>
-      <c r="G61" s="18" t="s">
+      <c r="G67" s="18" t="s">
         <v>417</v>
       </c>
-      <c r="H61" s="18" t="s">
+      <c r="H67" s="18" t="s">
         <v>418</v>
       </c>
-      <c r="I61" s="18" t="s">
+      <c r="I67" s="18" t="s">
         <v>419</v>
       </c>
-      <c r="J61" s="19" t="s">
+      <c r="J67" s="19" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="137" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="29"/>
-      <c r="B62" s="18" t="s">
+    <row r="68" spans="1:10" ht="137" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="30"/>
+      <c r="B68" s="18" t="s">
         <v>421</v>
       </c>
-      <c r="C62" s="18" t="s">
+      <c r="C68" s="18" t="s">
         <v>422</v>
       </c>
-      <c r="D62" s="18" t="s">
+      <c r="D68" s="18" t="s">
         <v>423</v>
       </c>
-      <c r="E62" s="18" t="s">
+      <c r="E68" s="18" t="s">
         <v>424</v>
       </c>
-      <c r="F62" s="18" t="s">
+      <c r="F68" s="18" t="s">
         <v>425</v>
       </c>
-      <c r="G62" s="18" t="s">
+      <c r="G68" s="18" t="s">
         <v>426</v>
       </c>
-      <c r="H62" s="18" t="s">
+      <c r="H68" s="18" t="s">
         <v>427</v>
       </c>
-      <c r="I62" s="18" t="s">
+      <c r="I68" s="18" t="s">
         <v>428</v>
       </c>
-      <c r="J62" s="19" t="s">
+      <c r="J68" s="19" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="176" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="20" t="s">
+    <row r="77" spans="1:10" ht="176" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="20" t="s">
         <v>430</v>
       </c>
-      <c r="B71" s="21" t="s">
+      <c r="B77" s="21" t="s">
         <v>431</v>
       </c>
-      <c r="C71" s="21" t="s">
+      <c r="C77" s="21" t="s">
         <v>432</v>
       </c>
-      <c r="D71" s="21" t="s">
+      <c r="D77" s="21" t="s">
         <v>433</v>
       </c>
-      <c r="E71" s="21" t="s">
+      <c r="E77" s="21" t="s">
         <v>434</v>
       </c>
-      <c r="F71" s="21" t="s">
+      <c r="F77" s="21" t="s">
         <v>435</v>
       </c>
-      <c r="G71" s="21" t="s">
+      <c r="G77" s="21" t="s">
         <v>436</v>
       </c>
-      <c r="H71" s="21" t="s">
+      <c r="H77" s="21" t="s">
         <v>437</v>
       </c>
-      <c r="I71" s="21" t="s">
+      <c r="I77" s="21" t="s">
         <v>438</v>
       </c>
-      <c r="J71" s="21"/>
+      <c r="J77" s="21"/>
     </row>
-    <row r="72" spans="1:10" ht="140" x14ac:dyDescent="0.25">
-      <c r="A72" s="20" t="s">
+    <row r="78" spans="1:10" ht="140" x14ac:dyDescent="0.25">
+      <c r="A78" s="20" t="s">
         <v>439</v>
       </c>
-      <c r="B72" s="21" t="s">
+      <c r="B78" s="21" t="s">
         <v>440</v>
       </c>
-      <c r="C72" s="21" t="s">
+      <c r="C78" s="21" t="s">
         <v>441</v>
       </c>
-      <c r="D72" s="21" t="s">
+      <c r="D78" s="21" t="s">
         <v>442</v>
       </c>
-      <c r="E72" s="21" t="s">
+      <c r="E78" s="21" t="s">
         <v>443</v>
       </c>
-      <c r="F72" s="21" t="s">
+      <c r="F78" s="21" t="s">
         <v>444</v>
       </c>
-      <c r="G72" s="21" t="s">
+      <c r="G78" s="21" t="s">
         <v>445</v>
       </c>
-      <c r="H72" s="21" t="s">
+      <c r="H78" s="21" t="s">
         <v>446</v>
       </c>
-      <c r="I72" s="21" t="s">
+      <c r="I78" s="21" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B76" s="19"/>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B82" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="32">
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
@@ -43877,28 +44530,31 @@
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A29:A30"/>
     <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A61:A62"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="A67:A68"/>
     <mergeCell ref="A48:A49"/>
     <mergeCell ref="A50:A51"/>
     <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A64:A65"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>